<commit_message>
adding parts list and motor calcs
</commit_message>
<xml_diff>
--- a/Documents/PartList.xlsx
+++ b/Documents/PartList.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jess/Documents/ece492/capstoneMovingTarget/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh HDD/Users/Jess/HDD Docs/ece492/capstoneMovingTarget/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{75E77CD4-3F93-024A-A3C7-0BBA4D899B57}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{75E77CD4-3F93-024A-A3C7-0BBA4D899B57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Part Name</t>
   </si>
@@ -65,39 +65,9 @@
     <t>V-SLOT Gantry Plate (20x80mm)</t>
   </si>
   <si>
-    <t>Solid V Wheel Kit</t>
-  </si>
-  <si>
     <t>https://makerparts.ca/products/v-slot-gantry-plates?variant=7103133764</t>
   </si>
   <si>
-    <t>https://makerparts.ca/products/solid-v-wheel-kit?variant=46466862031</t>
-  </si>
-  <si>
-    <t>Xtreme Solid V Wheel Kit</t>
-  </si>
-  <si>
-    <t>https://makerparts.ca/products/xtreme-solid-v-wheel-kit?variant=46466829839</t>
-  </si>
-  <si>
-    <t>Low Profile Screws M5 (25mm) - Single</t>
-  </si>
-  <si>
-    <t>https://makerparts.ca/products/low-profile-screws-m5?variant=19914942276</t>
-  </si>
-  <si>
-    <t>https://makerparts.ca/products/aluminum-spacer?variant=7102182084</t>
-  </si>
-  <si>
-    <t>Aluminum Spacer (6mm)</t>
-  </si>
-  <si>
-    <t>Eccentric Spacer</t>
-  </si>
-  <si>
-    <t>https://makerparts.ca/products/eccentric-spacer?variant=7101252484</t>
-  </si>
-  <si>
     <t>Total Price of All Parts</t>
   </si>
   <si>
@@ -189,6 +159,21 @@
   </si>
   <si>
     <t>(monochrome for openCV)</t>
+  </si>
+  <si>
+    <t>Wheels</t>
+  </si>
+  <si>
+    <t>V Slot Solid Wheel Kit</t>
+  </si>
+  <si>
+    <t>RoboShop Shipping</t>
+  </si>
+  <si>
+    <t>https://www.robotshop.com/ca/en/ratrig-solid-v-wheel-kit-normal-spacer.html</t>
+  </si>
+  <si>
+    <t>RobotShop</t>
   </si>
 </sst>
 </file>
@@ -256,19 +241,16 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -585,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8D26DF-C3B1-6F4B-BDA1-60184D1F1C9D}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,7 +587,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -627,8 +609,8 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>33</v>
+      <c r="A2" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -649,14 +631,14 @@
       <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="6"/>
+      <c r="M2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
@@ -666,24 +648,24 @@
         <v>8.67</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F33" si="0">D3*E3</f>
-        <v>17.34</v>
+        <f t="shared" ref="F3:F5" si="0">D3*E3</f>
+        <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="5">
         <f>SUM(F:F)</f>
-        <v>315.97999999999996</v>
-      </c>
-      <c r="N3" s="6"/>
+        <v>192.82</v>
+      </c>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -691,340 +673,290 @@
         <v>17.37</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>17.37</v>
+        <v>52.11</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="6"/>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1">
-        <v>7.18</v>
+        <v>29</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>50.26</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3"/>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1">
-        <v>9.91</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
+      <c r="C6"/>
+      <c r="D6" s="1"/>
       <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>49.55</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
+        <f>D6*E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3"/>
-      <c r="C7" t="s">
-        <v>18</v>
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D7" s="1">
-        <v>0.49</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="E7">
         <v>12</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>5.88</v>
+        <f t="shared" ref="F7:F8" si="1">D7*E7</f>
+        <v>57.239999999999995</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="3"/>
-      <c r="C8" t="s">
-        <v>21</v>
+      <c r="C8" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="D8" s="1">
-        <v>0.28999999999999998</v>
+        <v>11.7</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7399999999999998</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3"/>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2.95</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>17.700000000000003</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>11.7</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1">
-        <v>29</v>
+        <v>4.55</v>
       </c>
       <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <f>D10*E10</f>
+        <v>13.649999999999999</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C11"/>
-      <c r="D11" s="1"/>
       <c r="F11" s="1">
-        <f>D11*E11</f>
-        <v>0</v>
+        <f t="shared" ref="F11:F14" si="2">D11*E11</f>
+        <v>5.99</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4.55</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
       <c r="F12" s="1">
-        <f>D12*E12</f>
-        <v>13.649999999999999</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>27</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="1">
-        <v>5.99</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
       <c r="F13" s="1">
-        <f t="shared" ref="F13:F16" si="1">D13*E13</f>
-        <v>5.99</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>45</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>52</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3">
+        <v>19.12</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>D15*E15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>D16*E16</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
       <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="4">
-        <v>19.12</v>
+        <v>40</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3.07</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
         <f>D17*E17</f>
-        <v>38.24</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
-      <c r="F18" s="1">
-        <f>D18*E18</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1">
-        <v>3.07</v>
+        <v>32</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="1">
         <f>D19*E19</f>
-        <v>6.14</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>51</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <f>D20*E20</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="C21"/>
+      <c r="D21" s="1"/>
+      <c r="F21" s="1">
+        <f t="shared" ref="F21:F22" si="3">D21*E21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>38</v>
       </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="1">
-        <v>32</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <f>D21*E21</f>
-        <v>32</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D22" s="1">
-        <v>7.99</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1">
-        <f>D22*E22</f>
-        <v>7.99</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I22" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C23"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="1">
-        <f t="shared" ref="F23:F24" si="2">D23*E23</f>
-        <v>0</v>
-      </c>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="C24"/>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C25"/>
       <c r="D25" s="1"/>
       <c r="F25" s="1"/>
     </row>
@@ -1049,55 +981,26 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C30"/>
-      <c r="D30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C31"/>
-      <c r="D31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C32"/>
-      <c r="D32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C33"/>
-      <c r="D33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C34"/>
-      <c r="D34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E35" s="1"/>
+      <c r="E30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{37344D0B-419D-7C43-BF80-07E57AF5DC34}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{1299E937-74A9-644F-9C79-08E607AE1335}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{B999EE17-B151-7445-93B6-610942889291}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{76E10916-1072-9141-B2AC-AFB313A13D6F}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{F330B59B-47A3-124E-A3CE-7EBB73390C4A}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{F2B79C0A-0D52-7148-AD12-2A19EEEAB45C}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{F9983FC3-FEDF-D740-A6DD-2C259B9BABDA}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{C92AA364-3DBA-7D45-AA6F-9363FDC08B74}"/>
-    <hyperlink ref="G12" r:id="rId9" xr:uid="{0FA525A9-E7FB-6340-A5D8-808A34AFCBF2}"/>
-    <hyperlink ref="G17" r:id="rId10" xr:uid="{88CD4118-B647-DC45-A99D-89E88360A43A}"/>
-    <hyperlink ref="G21" r:id="rId11" xr:uid="{799D26E8-79B4-D14B-B4BF-7AED4539F8F6}"/>
-    <hyperlink ref="G22" r:id="rId12" xr:uid="{4A023F08-34AC-F84B-AB4B-098DF2844743}"/>
-    <hyperlink ref="G13" r:id="rId13" xr:uid="{23074A67-638D-1440-AFDB-B9A0622D0784}"/>
-    <hyperlink ref="G19" r:id="rId14" xr:uid="{C8AD481A-E734-7145-94DB-B2DE6EE16EBE}"/>
-    <hyperlink ref="G18" r:id="rId15" xr:uid="{44588527-05A9-3D48-B8E0-65FF8E17D299}"/>
-    <hyperlink ref="G24" r:id="rId16" xr:uid="{24A8444E-0A64-AF43-B730-4E8EFE109C22}"/>
+    <hyperlink ref="G10" r:id="rId4" xr:uid="{0FA525A9-E7FB-6340-A5D8-808A34AFCBF2}"/>
+    <hyperlink ref="G15" r:id="rId5" xr:uid="{88CD4118-B647-DC45-A99D-89E88360A43A}"/>
+    <hyperlink ref="G19" r:id="rId6" xr:uid="{799D26E8-79B4-D14B-B4BF-7AED4539F8F6}"/>
+    <hyperlink ref="G20" r:id="rId7" xr:uid="{4A023F08-34AC-F84B-AB4B-098DF2844743}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{23074A67-638D-1440-AFDB-B9A0622D0784}"/>
+    <hyperlink ref="G17" r:id="rId9" xr:uid="{C8AD481A-E734-7145-94DB-B2DE6EE16EBE}"/>
+    <hyperlink ref="G16" r:id="rId10" xr:uid="{44588527-05A9-3D48-B8E0-65FF8E17D299}"/>
+    <hyperlink ref="G22" r:id="rId11" xr:uid="{24A8444E-0A64-AF43-B730-4E8EFE109C22}"/>
+    <hyperlink ref="G7" r:id="rId12" xr:uid="{E4B34830-3A38-B446-84BF-F1636D9F699B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>